<commit_message>
Cambios en apariencia de tablas y diccionarios
</commit_message>
<xml_diff>
--- a/Catalogos_0412.xlsx
+++ b/Catalogos_0412.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hector.paredes\Desktop\datos abiertos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ProyectoProbCOVID\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E6758E-68E3-4BEB-9ABD-C72E2A5E22E3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10020" yWindow="270" windowWidth="12720" windowHeight="11925" tabRatio="911"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="911" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Catálogo ORIGEN" sheetId="3" r:id="rId1"/>
@@ -9103,7 +9104,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -9494,10 +9495,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9543,11 +9544,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9685,7 +9686,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9736,7 +9737,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9787,7 +9788,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9853,7 +9854,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9903,7 +9904,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A2:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9959,11 +9960,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10384,7 +10385,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C2502"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>